<commit_message>
se ajustan los script de las HU de consultas de pagos
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/consultadepagos/consultadepagos.xlsx
+++ b/SVP/src/test/resources/datadriven/consultadepagos/consultadepagos.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
     <sheet name="Datos2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -19,8 +19,46 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Usuario</author>
+  </authors>
+  <commentList>
+    <comment ref="K1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ingresar cuatro "*" mas los ultimos 4 digitos de la tarjeta de credito y separar por ",". Ejemplo ****0175, ****0556</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ingresar un "*" mas los ultimos 4 digitos del credito y separar por ",". Ejemplo *1234, *3456</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
   <si>
     <t>idCaso</t>
   </si>
@@ -158,13 +196,28 @@
   </si>
   <si>
     <t>9</t>
+  </si>
+  <si>
+    <t>tarjetasCredito</t>
+  </si>
+  <si>
+    <t>creditos</t>
+  </si>
+  <si>
+    <t>mensajeRespuesta</t>
+  </si>
+  <si>
+    <t>escenario</t>
+  </si>
+  <si>
+    <t>mensajeRespuesta_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -178,8 +231,26 @@
       <name val="Mic Shell Dlg"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Mic Shell Dlg"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,8 +269,14 @@
         <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -222,11 +299,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -244,6 +332,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -613,11 +704,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -632,9 +723,12 @@
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" customWidth="1"/>
     <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" customWidth="1"/>
+    <col min="14" max="14" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -665,8 +759,23 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -687,8 +796,13 @@
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -709,8 +823,13 @@
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -733,8 +852,13 @@
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -755,8 +879,13 @@
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
@@ -779,8 +908,13 @@
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -801,8 +935,13 @@
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -823,8 +962,13 @@
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="3" t="s">
         <v>44</v>
       </c>
@@ -845,8 +989,13 @@
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="3" t="s">
         <v>45</v>
       </c>
@@ -867,10 +1016,16 @@
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="3"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>

<commit_message>
Se realiza implementación de scripts de la HU de consultas de pagos con los cambios pasados a qa hasta la fecha
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/consultadepagos/consultadepagos.xlsx
+++ b/SVP/src/test/resources/datadriven/consultadepagos/consultadepagos.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="52">
   <si>
     <t>idCaso</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Hola</t>
   </si>
   <si>
-    <t>OSVPPRU11</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -114,12 +111,6 @@
     <t>Usuario o clave inválida. Inténtalo nuevamente</t>
   </si>
   <si>
-    <t>52269682</t>
-  </si>
-  <si>
-    <t>OSVPPRU10</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -211,6 +202,18 @@
   </si>
   <si>
     <t>mensajeRespuesta_2</t>
+  </si>
+  <si>
+    <t>pruebaavance01</t>
+  </si>
+  <si>
+    <t>*4676</t>
+  </si>
+  <si>
+    <t>Validar pagos  de una tarjeta de crédito</t>
+  </si>
+  <si>
+    <t>¡LO QUIERO!</t>
   </si>
 </sst>
 </file>
@@ -314,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -335,6 +338,9 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -708,7 +714,7 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -719,13 +725,14 @@
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
     <col min="5" max="5" width="139.28515625" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" customWidth="1"/>
     <col min="10" max="10" width="15.140625" customWidth="1"/>
     <col min="11" max="11" width="17.85546875" customWidth="1"/>
     <col min="13" max="13" width="19.42578125" customWidth="1"/>
     <col min="14" max="14" width="24.5703125" customWidth="1"/>
+    <col min="15" max="15" width="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -760,19 +767,19 @@
         <v>9</v>
       </c>
       <c r="K1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -784,27 +791,29 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="E2" s="3"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="H2" s="5">
         <v>1234</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="3"/>
-      <c r="K2" s="5"/>
+      <c r="K2" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="O2" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
@@ -816,7 +825,7 @@
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="5">
         <v>1234</v>
@@ -831,21 +840,17 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="H4" s="5">
         <v>1234</v>
@@ -855,24 +860,26 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="N4" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="O4" s="5"/>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H5" s="5">
         <v>4567</v>
@@ -887,21 +894,21 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H6" s="5">
         <v>1234</v>
@@ -916,19 +923,19 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H7" s="5">
         <v>1234</v>
@@ -943,18 +950,18 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="5">
@@ -970,18 +977,18 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="5">
@@ -997,18 +1004,18 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="5">
@@ -1102,12 +1109,12 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1116,7 +1123,7 @@
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1124,23 +1131,23 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H3" s="5">
         <v>1234</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1148,12 +1155,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -1162,7 +1169,7 @@
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1170,23 +1177,23 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H5" s="5">
         <v>1234</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="41.25" customHeight="1">
@@ -1194,34 +1201,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H6" s="5">
         <v>1234</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="5"/>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -1230,7 +1237,7 @@
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1238,12 +1245,12 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -1252,7 +1259,7 @@
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1260,12 +1267,12 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1274,7 +1281,7 @@
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1282,12 +1289,12 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -1296,7 +1303,7 @@
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se implementan scripts correspondientes a la HU de consultas de pago
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/consultadepagos/consultadepagos.xlsx
+++ b/SVP/src/test/resources/datadriven/consultadepagos/consultadepagos.xlsx
@@ -47,7 +47,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Ingresar un "*" mas los ultimos 4 digitos del credito y separar por ",". Ejemplo *1234, *3456</t>
         </r>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
   <si>
     <t>idCaso</t>
   </si>
@@ -96,45 +96,24 @@
     <t>Acierto</t>
   </si>
   <si>
-    <t>Hola</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
-    <t>chipote25</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
-    <t>Usuario o clave inválida. Inténtalo nuevamente</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
     <t>Alterno</t>
   </si>
   <si>
-    <t>OSVPPRU06</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
-    <t>La clave que usas en el cajero está bloqueada. Debes activarla en la Sucursal Física. Para mayor información comunícate con la Sucursal Telefónica.</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
-    <t>OOMAP12</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
@@ -207,20 +186,47 @@
     <t>pruebaavance01</t>
   </si>
   <si>
-    <t>*4676</t>
-  </si>
-  <si>
     <t>Validar pagos  de una tarjeta de crédito</t>
   </si>
   <si>
     <t>¡LO QUIERO!</t>
+  </si>
+  <si>
+    <t>Validar usuario sin crédito</t>
+  </si>
+  <si>
+    <t>OSVPPRU15</t>
+  </si>
+  <si>
+    <t>Validar pagos de créditos.</t>
+  </si>
+  <si>
+    <t>Los productos están ocultos, puedes habilitarlos nuevamente en la opción "Productos/ Administrar productos propios".</t>
+  </si>
+  <si>
+    <t>USUARIOTODO1</t>
+  </si>
+  <si>
+    <t>****0175,****0556,****9636</t>
+  </si>
+  <si>
+    <t>USUCFEI01</t>
+  </si>
+  <si>
+    <t>****7618</t>
+  </si>
+  <si>
+    <t>OSVPPRU02</t>
+  </si>
+  <si>
+    <t>PRUEBAICDSC1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -246,11 +252,35 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Mic Shell Dlg"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Mic Shell Dlg"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF808285"/>
+      <name val="Open Sans"/>
     </font>
   </fonts>
   <fills count="5">
@@ -314,10 +344,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -342,8 +373,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -711,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -723,14 +762,15 @@
     <col min="2" max="2" width="11.140625" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="139.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" customWidth="1"/>
     <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" customWidth="1"/>
+    <col min="11" max="11" width="27.28515625" customWidth="1"/>
+    <col min="12" max="12" width="28.42578125" customWidth="1"/>
+    <col min="13" max="13" width="110.42578125" customWidth="1"/>
     <col min="14" max="14" width="24.5703125" customWidth="1"/>
     <col min="15" max="15" width="35" customWidth="1"/>
   </cols>
@@ -767,19 +807,19 @@
         <v>9</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -794,7 +834,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H2" s="5">
         <v>1234</v>
@@ -802,30 +842,28 @@
       <c r="I2" s="5"/>
       <c r="J2" s="3"/>
       <c r="K2" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="E3" s="3"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="H3" s="5">
         <v>1234</v>
@@ -833,14 +871,18 @@
       <c r="I3" s="5"/>
       <c r="J3" s="3"/>
       <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
+      <c r="L3" s="4">
+        <v>29281025315</v>
+      </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
+      <c r="O3" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>11</v>
@@ -850,7 +892,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="H4" s="5">
         <v>1234</v>
@@ -861,29 +903,25 @@
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="O4" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="E5" s="3"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="5">
-        <v>4567</v>
-      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="3"/>
       <c r="K5" s="5"/>
@@ -892,23 +930,19 @@
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" ht="18.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="H6" s="5">
         <v>1234</v>
@@ -917,25 +951,25 @@
       <c r="J6" s="3"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
+      <c r="M6" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="E7" s="3"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="H7" s="5">
         <v>1234</v>
@@ -944,26 +978,28 @@
       <c r="J7" s="3"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
+      <c r="M7" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="E8" s="3"/>
       <c r="F8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="H8" s="5">
         <v>1234</v>
       </c>
@@ -971,24 +1007,24 @@
       <c r="J8" s="3"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
+      <c r="M8" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="E9" s="3"/>
       <c r="F9" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="5">
@@ -1004,18 +1040,16 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="E10" s="3"/>
       <c r="F10" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="5">
@@ -1024,10 +1058,35 @@
       <c r="I10" s="5"/>
       <c r="J10" s="3"/>
       <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
+      <c r="L10" s="14"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="13">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="5">
+        <v>1234</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1109,12 +1168,12 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1123,7 +1182,7 @@
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1131,23 +1190,23 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="H3" s="5">
         <v>1234</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1155,12 +1214,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -1169,7 +1228,7 @@
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1177,23 +1236,23 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H5" s="5">
         <v>1234</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="41.25" customHeight="1">
@@ -1201,34 +1260,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="H6" s="5">
         <v>1234</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="5"/>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -1237,7 +1296,7 @@
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1245,12 +1304,12 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -1259,7 +1318,7 @@
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1267,12 +1326,12 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1281,7 +1340,7 @@
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1289,12 +1348,12 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -1303,7 +1362,7 @@
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se implementa los scripts de consulta de pagos en un 80% con respecto a las funcionalidas de la HU
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/consultadepagos/consultadepagos.xlsx
+++ b/SVP/src/test/resources/datadriven/consultadepagos/consultadepagos.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="59">
   <si>
     <t>idCaso</t>
   </si>
@@ -189,9 +189,6 @@
     <t>Validar pagos  de una tarjeta de crédito</t>
   </si>
   <si>
-    <t>¡LO QUIERO!</t>
-  </si>
-  <si>
     <t>Validar usuario sin crédito</t>
   </si>
   <si>
@@ -204,12 +201,6 @@
     <t>Los productos están ocultos, puedes habilitarlos nuevamente en la opción "Productos/ Administrar productos propios".</t>
   </si>
   <si>
-    <t>USUARIOTODO1</t>
-  </si>
-  <si>
-    <t>****0175,****0556,****9636</t>
-  </si>
-  <si>
     <t>USUCFEI01</t>
   </si>
   <si>
@@ -220,13 +211,37 @@
   </si>
   <si>
     <t>PRUEBAICDSC1</t>
+  </si>
+  <si>
+    <t>Consulta de pagos de tarjetas de credito (usuario con tarjetas de creditos ocultas)</t>
+  </si>
+  <si>
+    <t>Consulta de pagos de credito (usuario con creditos ocultos)</t>
+  </si>
+  <si>
+    <t>Consulta de pagos de credito y tarjetas creditos (creditos y tarjetas creditos ocultos)</t>
+  </si>
+  <si>
+    <t>Consulta de pagos de tarjetas de credito exitoso sin fecha</t>
+  </si>
+  <si>
+    <t>****5949,****1123,****2495</t>
+  </si>
+  <si>
+    <t>29281025315</t>
+  </si>
+  <si>
+    <t>Validar usuario con tarjetas y créditos</t>
+  </si>
+  <si>
+    <t>LO QUIERO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -276,11 +291,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF808285"/>
-      <name val="Open Sans"/>
     </font>
   </fonts>
   <fills count="5">
@@ -348,7 +358,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -375,11 +385,10 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -752,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -768,11 +777,11 @@
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" customWidth="1"/>
     <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="11" width="27.28515625" customWidth="1"/>
-    <col min="12" max="12" width="28.42578125" customWidth="1"/>
+    <col min="11" max="11" width="28.140625" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" customWidth="1"/>
     <col min="13" max="13" width="110.42578125" customWidth="1"/>
-    <col min="14" max="14" width="24.5703125" customWidth="1"/>
-    <col min="15" max="15" width="35" customWidth="1"/>
+    <col min="14" max="14" width="31.7109375" customWidth="1"/>
+    <col min="15" max="15" width="85.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -834,7 +843,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H2" s="5">
         <v>1234</v>
@@ -842,7 +851,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="3"/>
       <c r="K2" s="5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
@@ -863,7 +872,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" s="5">
         <v>1234</v>
@@ -871,13 +880,13 @@
       <c r="I3" s="5"/>
       <c r="J3" s="3"/>
       <c r="K3" s="5"/>
-      <c r="L3" s="4">
-        <v>29281025315</v>
+      <c r="L3" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -892,7 +901,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H4" s="5">
         <v>1234</v>
@@ -903,10 +912,10 @@
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="O4" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -952,10 +961,12 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="O6" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="3" t="s">
@@ -969,7 +980,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H7" s="5">
         <v>1234</v>
@@ -979,10 +990,12 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
+      <c r="O7" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="3" t="s">
@@ -998,7 +1011,7 @@
         <v>19</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H8" s="5">
         <v>1234</v>
@@ -1007,11 +1020,13 @@
       <c r="J8" s="3"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="12" t="s">
-        <v>47</v>
+      <c r="M8" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
+      <c r="O8" s="5" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="3" t="s">
@@ -1051,20 +1066,28 @@
       <c r="F10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="4"/>
+      <c r="G10" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="H10" s="5">
         <v>1234</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="14"/>
+      <c r="K10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
+      <c r="O10" s="5" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="13">
+      <c r="A11" s="12">
         <v>10</v>
       </c>
       <c r="B11" s="5"/>
@@ -1073,7 +1096,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H11" s="5">
         <v>1234</v>
@@ -1081,12 +1104,14 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
+      <c r="O11" s="5" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
se termina la implementación de los scripts de la HU consulta de pagos
</commit_message>
<xml_diff>
--- a/SVP/src/test/resources/datadriven/consultadepagos/consultadepagos.xlsx
+++ b/SVP/src/test/resources/datadriven/consultadepagos/consultadepagos.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="63">
   <si>
     <t>idCaso</t>
   </si>
@@ -235,6 +235,18 @@
   </si>
   <si>
     <t>mensajeRespuestaDos</t>
+  </si>
+  <si>
+    <t>OSVPPRU30</t>
+  </si>
+  <si>
+    <t>LA QUIERO</t>
+  </si>
+  <si>
+    <t>Validar usuario sin tarjetas y sin créditos</t>
+  </si>
+  <si>
+    <t>Validar usuario sin tarjeta de crédito.</t>
   </si>
 </sst>
 </file>
@@ -358,7 +370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -389,6 +401,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -762,7 +777,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -929,15 +944,23 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
+      <c r="G5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1234</v>
+      </c>
       <c r="I5" s="5"/>
       <c r="J5" s="3"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
+      <c r="N5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="6" spans="1:15" ht="18.75" customHeight="1">
       <c r="A6" s="3" t="s">
@@ -1041,7 +1064,9 @@
       <c r="F9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="H9" s="5">
         <v>1234</v>
       </c>
@@ -1049,9 +1074,15 @@
       <c r="J9" s="3"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
+      <c r="M9" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="3" t="s">

</xml_diff>